<commit_message>
add server security state machine diagram for extra credit
</commit_message>
<xml_diff>
--- a/questions/Server Command Table A8.xlsx
+++ b/questions/Server Command Table A8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bjornnelson/SimplicityStudio/v5_workspace/ecen5823-assignment8-bjornhnelson/questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FF77DE-233F-934F-A199-0B27437A6DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49C486E-329E-A141-B559-ABAC7F8F35D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -234,9 +234,6 @@
 There is no indication currently in-flight</t>
   </si>
   <si>
-    <t>For this assignment these are our events from LETIMER0 and the I2C transfers. A8 new part: handle passkey sequence and writing button state to GATT database</t>
-  </si>
-  <si>
     <t>sl_bt_evt_system_soft_timer_id</t>
   </si>
   <si>
@@ -280,6 +277,9 @@
   </si>
   <si>
     <t>sl_bt_gatt_server_write_attribute_value(</t>
+  </si>
+  <si>
+    <t>For this assignment these are our events from LETIMER0 and the I2C transfers. A8 new part: handle passkey sequence, writing button state to GATT database, sending button state indications</t>
   </si>
 </sst>
 </file>
@@ -553,6 +553,55 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>84666</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>732366</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>1972732</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD466C28-BE32-3449-87E0-B131D5BD54E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19642666" y="5384799"/>
+          <a:ext cx="6388100" cy="4038600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1633,8 +1682,8 @@
   </sheetPr>
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D8" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F12" zoomScale="75" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="15.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1906,10 +1955,10 @@
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="22" t="s">
         <v>63</v>
-      </c>
-      <c r="F21" s="22" t="s">
-        <v>48</v>
       </c>
       <c r="G21" s="24" t="s">
         <v>47</v>
@@ -1918,17 +1967,17 @@
     <row r="22" spans="1:7" ht="169" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="25" t="s">
         <v>49</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>50</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G22" s="24"/>
     </row>
@@ -2005,14 +2054,14 @@
     <row r="29" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
       <c r="B29" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F29" s="27"/>
       <c r="G29" s="9"/>
@@ -2028,16 +2077,16 @@
     <row r="31" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9"/>
       <c r="B31" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="27"/>
       <c r="G31" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
@@ -2051,16 +2100,16 @@
     <row r="33" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
       <c r="B33" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
       <c r="F33" s="27"/>
       <c r="G33" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
@@ -2075,16 +2124,16 @@
     <row r="35" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9"/>
       <c r="B35" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
       <c r="F35" s="27"/>
       <c r="G35" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
@@ -2105,5 +2154,6 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>